<commit_message>
Updates actual Release Planning Excel spreadsheet
</commit_message>
<xml_diff>
--- a/Documentation/Release Planning.xlsx
+++ b/Documentation/Release Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19980" windowHeight="20040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Breakdown " sheetId="1" r:id="rId1"/>
@@ -678,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -780,6 +780,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1061,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BO368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AD17" sqref="AD17"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="125" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2672,7 +2687,7 @@
       <c r="BD22" s="11"/>
       <c r="BE22" s="11"/>
     </row>
-    <row r="23" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>4.0999999999999996</v>
       </c>
@@ -2733,7 +2748,7 @@
       <c r="BD23" s="11"/>
       <c r="BE23" s="11"/>
     </row>
-    <row r="24" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>29</v>
       </c>
@@ -2764,7 +2779,7 @@
       <c r="Z24" s="11"/>
       <c r="AA24" s="11"/>
       <c r="AB24" s="11"/>
-      <c r="AC24" s="11"/>
+      <c r="AC24" s="37"/>
       <c r="AD24" s="12"/>
       <c r="AE24" s="11"/>
       <c r="AF24" s="11"/>
@@ -2977,7 +2992,7 @@
       <c r="BD27" s="11"/>
       <c r="BE27" s="11"/>
     </row>
-    <row r="28" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>54</v>
       </c>
@@ -3007,15 +3022,15 @@
       <c r="Y28" s="12"/>
       <c r="Z28" s="12"/>
       <c r="AA28" s="12"/>
-      <c r="AB28" s="12"/>
+      <c r="AB28" s="38"/>
       <c r="AC28" s="12"/>
       <c r="AD28" s="12"/>
-      <c r="AE28" s="12"/>
-      <c r="AH28" s="11"/>
-      <c r="AI28" s="11"/>
-      <c r="AJ28" s="11"/>
-      <c r="AK28" s="11"/>
-      <c r="AL28" s="11"/>
+      <c r="AE28" s="38"/>
+      <c r="AH28" s="37"/>
+      <c r="AI28" s="37"/>
+      <c r="AJ28" s="37"/>
+      <c r="AK28" s="37"/>
+      <c r="AL28" s="37"/>
       <c r="AM28" s="11"/>
       <c r="AN28" s="11"/>
       <c r="AO28" s="11"/>
@@ -3036,7 +3051,7 @@
       <c r="BD28" s="11"/>
       <c r="BE28" s="11"/>
     </row>
-    <row r="29" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>55</v>
       </c>
@@ -3072,9 +3087,10 @@
       <c r="AE29" s="12"/>
       <c r="AF29" s="12"/>
       <c r="AG29" s="12"/>
-      <c r="AH29" s="12"/>
+      <c r="AH29" s="38"/>
+      <c r="AI29" s="39"/>
       <c r="AK29" s="11"/>
-      <c r="AL29" s="11"/>
+      <c r="AL29" s="37"/>
       <c r="AM29" s="11"/>
       <c r="AN29" s="11"/>
       <c r="AO29" s="11"/>
@@ -3156,7 +3172,7 @@
       <c r="BD30" s="11"/>
       <c r="BE30" s="11"/>
     </row>
-    <row r="31" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>56</v>
       </c>
@@ -3217,7 +3233,7 @@
       <c r="BD31" s="11"/>
       <c r="BE31" s="11"/>
     </row>
-    <row r="32" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>57</v>
       </c>
@@ -3257,7 +3273,7 @@
       <c r="AI32" s="11"/>
       <c r="AJ32" s="11"/>
       <c r="AK32" s="11"/>
-      <c r="AL32" s="11"/>
+      <c r="AL32" s="37"/>
       <c r="AM32" s="11"/>
       <c r="AN32" s="11"/>
       <c r="AO32" s="11"/>
@@ -3278,7 +3294,7 @@
       <c r="BD32" s="11"/>
       <c r="BE32" s="11"/>
     </row>
-    <row r="33" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>4.4000000000000004</v>
       </c>
@@ -3339,7 +3355,7 @@
       <c r="BD33" s="11"/>
       <c r="BE33" s="11"/>
     </row>
-    <row r="34" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>37</v>
       </c>
@@ -3376,9 +3392,9 @@
       <c r="AF34" s="11"/>
       <c r="AG34" s="11"/>
       <c r="AH34" s="11"/>
-      <c r="AI34" s="11"/>
-      <c r="AJ34" s="11"/>
-      <c r="AK34" s="11"/>
+      <c r="AI34" s="37"/>
+      <c r="AJ34" s="37"/>
+      <c r="AK34" s="37"/>
       <c r="AL34" s="11"/>
       <c r="AM34" s="11"/>
       <c r="AN34" s="11"/>
@@ -3400,7 +3416,7 @@
       <c r="BD34" s="11"/>
       <c r="BE34" s="11"/>
     </row>
-    <row r="35" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>38</v>
       </c>
@@ -3440,7 +3456,7 @@
       <c r="AI35" s="11"/>
       <c r="AJ35" s="11"/>
       <c r="AK35" s="11"/>
-      <c r="AL35" s="11"/>
+      <c r="AL35" s="37"/>
       <c r="AM35" s="11"/>
       <c r="AN35" s="11"/>
       <c r="AO35" s="11"/>
@@ -3461,7 +3477,7 @@
       <c r="BD35" s="11"/>
       <c r="BE35" s="11"/>
     </row>
-    <row r="36" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>4.5</v>
       </c>
@@ -3502,7 +3518,7 @@
       <c r="AJ36" s="11"/>
       <c r="AK36" s="11"/>
       <c r="AL36" s="11"/>
-      <c r="AM36" s="11"/>
+      <c r="AM36" s="43"/>
       <c r="AN36" s="11"/>
       <c r="AO36" s="11"/>
       <c r="AP36" s="11"/>
@@ -3522,7 +3538,7 @@
       <c r="BD36" s="11"/>
       <c r="BE36" s="11"/>
     </row>
-    <row r="37" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>45</v>
       </c>
@@ -3561,9 +3577,9 @@
       <c r="AH37" s="12"/>
       <c r="AI37" s="11"/>
       <c r="AJ37" s="11"/>
-      <c r="AK37" s="11"/>
-      <c r="AL37" s="11"/>
-      <c r="AM37" s="11"/>
+      <c r="AK37" s="37"/>
+      <c r="AL37" s="37"/>
+      <c r="AM37" s="43"/>
       <c r="AN37" s="11"/>
       <c r="AO37" s="11"/>
       <c r="AP37" s="11"/>
@@ -3583,7 +3599,7 @@
       <c r="BD37" s="11"/>
       <c r="BE37" s="11"/>
     </row>
-    <row r="38" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>4.5999999999999996</v>
       </c>
@@ -3644,7 +3660,7 @@
       <c r="BD38" s="11"/>
       <c r="BE38" s="11"/>
     </row>
-    <row r="39" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>46</v>
       </c>
@@ -3680,11 +3696,11 @@
       <c r="AE39" s="11"/>
       <c r="AF39" s="11"/>
       <c r="AG39" s="11"/>
-      <c r="AH39" s="11"/>
-      <c r="AI39" s="11"/>
-      <c r="AJ39" s="11"/>
-      <c r="AK39" s="11"/>
-      <c r="AL39" s="11"/>
+      <c r="AH39" s="40"/>
+      <c r="AI39" s="37"/>
+      <c r="AJ39" s="41"/>
+      <c r="AK39" s="37"/>
+      <c r="AL39" s="42"/>
       <c r="AM39" s="11"/>
       <c r="AN39" s="11"/>
       <c r="AO39" s="11"/>
@@ -3705,7 +3721,7 @@
       <c r="BD39" s="11"/>
       <c r="BE39" s="11"/>
     </row>
-    <row r="40" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>49</v>
       </c>
@@ -3745,7 +3761,7 @@
       <c r="AI40" s="11"/>
       <c r="AJ40" s="11"/>
       <c r="AK40" s="11"/>
-      <c r="AL40" s="11"/>
+      <c r="AL40" s="37"/>
       <c r="AM40" s="11"/>
       <c r="AN40" s="11"/>
       <c r="AO40" s="11"/>
@@ -3766,7 +3782,7 @@
       <c r="BD40" s="11"/>
       <c r="BE40" s="11"/>
     </row>
-    <row r="41" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>4.7</v>
       </c>
@@ -3827,7 +3843,7 @@
       <c r="BD41" s="11"/>
       <c r="BE41" s="11"/>
     </row>
-    <row r="42" spans="1:57" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:57" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>47</v>
       </c>
@@ -3867,8 +3883,8 @@
       <c r="AI42" s="11"/>
       <c r="AJ42" s="11"/>
       <c r="AK42" s="11"/>
-      <c r="AL42" s="11"/>
-      <c r="AM42" s="11"/>
+      <c r="AL42" s="37"/>
+      <c r="AM42" s="43"/>
       <c r="AN42" s="11"/>
       <c r="AO42" s="11"/>
       <c r="AP42" s="11"/>
@@ -4884,10 +4900,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D40"/>
+  <dimension ref="A2:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D40"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4964,119 +4980,119 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D10" s="36"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D11" s="36"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D12" s="36"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D13" s="36">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D14" s="36"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="C15" t="s">
-        <v>142</v>
-      </c>
-      <c r="D15" s="36"/>
+        <v>140</v>
+      </c>
+      <c r="D15" s="36">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
-      </c>
-      <c r="D16" s="36" t="s">
-        <v>166</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="D16" s="36"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D17" s="36"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" s="36"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>118</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>145</v>
       </c>
-      <c r="D18" s="36"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="C19" t="s">
-        <v>146</v>
-      </c>
-      <c r="D19" s="36">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="C20" t="s">
-        <v>147</v>
-      </c>
-      <c r="D20" s="36">
-        <v>15</v>
-      </c>
+      <c r="D20" s="36"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="35" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C21" t="s">
-        <v>153</v>
-      </c>
-      <c r="D21" s="36"/>
+        <v>147</v>
+      </c>
+      <c r="D21" s="36">
+        <v>15</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="35" t="s">
@@ -5106,73 +5122,64 @@
       <c r="D24" s="36"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D25" s="36"/>
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" t="s">
+        <v>163</v>
+      </c>
+      <c r="D25" s="36">
+        <v>11</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="33" t="s">
+      <c r="D26" s="36"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="36"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27" t="s">
-        <v>135</v>
-      </c>
       <c r="D27" s="36"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>114</v>
-      </c>
-      <c r="C28" t="s">
-        <v>138</v>
-      </c>
-      <c r="D28" s="36">
-        <v>5</v>
-      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="35" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D29" s="36">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" t="s">
+        <v>148</v>
+      </c>
+      <c r="D30" s="36">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>149</v>
       </c>
-      <c r="D30" s="36" t="s">
+      <c r="D31" s="36" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>123</v>
-      </c>
-      <c r="C31" t="s">
-        <v>150</v>
-      </c>
-      <c r="D31" s="36">
-        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D32" s="36">
         <v>15</v>
@@ -5180,83 +5187,92 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C33" t="s">
-        <v>152</v>
-      </c>
-      <c r="D33" s="36" t="s">
-        <v>165</v>
+        <v>151</v>
+      </c>
+      <c r="D33" s="36">
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="C34" t="s">
-        <v>157</v>
-      </c>
-      <c r="D34" s="36"/>
+        <v>152</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>102</v>
+      <c r="B35" s="35" t="s">
+        <v>126</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
-      </c>
-      <c r="D35" s="36">
-        <v>24</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="D35" s="36"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C36" t="s">
-        <v>159</v>
-      </c>
-      <c r="D36" s="36">
-        <v>1</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="D36" s="36"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C37" t="s">
-        <v>160</v>
-      </c>
-      <c r="D37" s="36"/>
+        <v>158</v>
+      </c>
+      <c r="D37" s="36">
+        <v>24</v>
+      </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>161</v>
-      </c>
-      <c r="D38" s="36"/>
+        <v>159</v>
+      </c>
+      <c r="D38" s="36">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C39" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D39" s="36"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C40" t="s">
-        <v>163</v>
-      </c>
-      <c r="D40" s="36">
-        <v>11</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="D40" s="36"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>